<commit_message>
WK3 Pro's roll up
</commit_message>
<xml_diff>
--- a/data/prosrollup.xlsx
+++ b/data/prosrollup.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Settings" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="128">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -360,6 +361,33 @@
   </si>
   <si>
     <t xml:space="preserve">Pros Roll Up Week 2 - DQ’ed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pros Roll Up Week 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 May 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pros Roll Up Week 3 - Stableford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simon Whitaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brian Combe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connor Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jordan Walker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nigel Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James Holman</t>
   </si>
   <si>
     <t xml:space="preserve">Key</t>
@@ -508,7 +536,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -537,6 +565,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -627,6 +659,46 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -886,10 +958,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K68"/>
+  <dimension ref="A1:K92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L49" activeCellId="0" sqref="L49"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N54" activeCellId="0" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -898,7 +970,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="17.19"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="8.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="28.83"/>
@@ -907,7 +979,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="3" width="10.16"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -938,1779 +1010,2424 @@
       <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="11" t="n">
+      <c r="E2" s="12" t="n">
         <v>10</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="11" t="n">
+      <c r="G2" s="12" t="n">
         <v>30</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="11" t="n">
+      <c r="E3" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="11" t="n">
+      <c r="E4" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="11" t="n">
+      <c r="E5" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="12" t="s">
+      <c r="G5" s="11"/>
+      <c r="H5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="11" t="n">
+      <c r="E6" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="12" t="s">
+      <c r="G6" s="11"/>
+      <c r="H6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="14" t="s">
+      <c r="E7" s="18"/>
+      <c r="F7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="18" t="s">
+      <c r="G7" s="17"/>
+      <c r="H7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="14" t="s">
+      <c r="E8" s="18"/>
+      <c r="F8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="18" t="s">
+      <c r="G8" s="17"/>
+      <c r="H8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="14" t="s">
+      <c r="E9" s="18"/>
+      <c r="F9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="18" t="s">
+      <c r="G9" s="17"/>
+      <c r="H9" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="14" t="s">
+      <c r="E10" s="18"/>
+      <c r="F10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="18" t="s">
+      <c r="G10" s="17"/>
+      <c r="H10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="14" t="s">
+      <c r="E11" s="18"/>
+      <c r="F11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="18" t="s">
+      <c r="G11" s="17"/>
+      <c r="H11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16" t="s">
+      <c r="B12" s="16"/>
+      <c r="C12" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="14" t="s">
+      <c r="E12" s="18"/>
+      <c r="F12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="18" t="s">
+      <c r="G12" s="17"/>
+      <c r="H12" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="19" t="s">
+      <c r="J12" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16" t="s">
+      <c r="B13" s="16"/>
+      <c r="C13" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="14" t="s">
+      <c r="E13" s="18"/>
+      <c r="F13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="18" t="s">
+      <c r="G13" s="17"/>
+      <c r="H13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="19" t="s">
+      <c r="J13" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16" t="s">
+      <c r="B14" s="16"/>
+      <c r="C14" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="14" t="s">
+      <c r="E14" s="18"/>
+      <c r="F14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="18" t="s">
+      <c r="G14" s="17"/>
+      <c r="H14" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="19" t="s">
+      <c r="J14" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="16" t="s">
+      <c r="B15" s="16"/>
+      <c r="C15" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="14" t="s">
+      <c r="E15" s="18"/>
+      <c r="F15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="18" t="s">
+      <c r="G15" s="17"/>
+      <c r="H15" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J15" s="19" t="s">
+      <c r="J15" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="16" t="s">
+      <c r="B16" s="16"/>
+      <c r="C16" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="14" t="s">
+      <c r="E16" s="18"/>
+      <c r="F16" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="18" t="s">
+      <c r="G16" s="17"/>
+      <c r="H16" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="I16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16" t="s">
+      <c r="B17" s="16"/>
+      <c r="C17" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="14" t="s">
+      <c r="E17" s="18"/>
+      <c r="F17" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="18" t="s">
+      <c r="G17" s="17"/>
+      <c r="H17" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16" t="s">
+      <c r="B18" s="16"/>
+      <c r="C18" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="14" t="s">
+      <c r="E18" s="18"/>
+      <c r="F18" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="18" t="s">
+      <c r="G18" s="18"/>
+      <c r="H18" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16" t="s">
+      <c r="B19" s="16"/>
+      <c r="C19" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="14" t="s">
+      <c r="E19" s="18"/>
+      <c r="F19" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="17"/>
-      <c r="H19" s="18" t="s">
+      <c r="G19" s="18"/>
+      <c r="H19" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="I19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J19" s="19" t="s">
+      <c r="J19" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="16" t="s">
+      <c r="B20" s="16"/>
+      <c r="C20" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="14" t="s">
+      <c r="E20" s="18"/>
+      <c r="F20" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="16"/>
-      <c r="H20" s="18" t="s">
+      <c r="G20" s="17"/>
+      <c r="H20" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="14" t="s">
+      <c r="I20" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J20" s="19" t="s">
+      <c r="J20" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16" t="s">
+      <c r="B21" s="16"/>
+      <c r="C21" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="14" t="s">
+      <c r="E21" s="18"/>
+      <c r="F21" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="16"/>
-      <c r="H21" s="18" t="s">
+      <c r="G21" s="17"/>
+      <c r="H21" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I21" s="14" t="s">
+      <c r="I21" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J21" s="19" t="s">
+      <c r="J21" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16" t="s">
+      <c r="B22" s="16"/>
+      <c r="C22" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="14" t="s">
+      <c r="E22" s="18"/>
+      <c r="F22" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="16"/>
-      <c r="H22" s="18" t="s">
+      <c r="G22" s="17"/>
+      <c r="H22" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="14" t="s">
+      <c r="I22" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="16" t="s">
+      <c r="B23" s="16"/>
+      <c r="C23" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="14" t="s">
+      <c r="E23" s="18"/>
+      <c r="F23" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="16"/>
-      <c r="H23" s="18" t="s">
+      <c r="G23" s="17"/>
+      <c r="H23" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J23" s="19" t="s">
+      <c r="J23" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="16" t="s">
+      <c r="B24" s="16"/>
+      <c r="C24" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="14" t="s">
+      <c r="E24" s="18"/>
+      <c r="F24" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="16"/>
-      <c r="H24" s="18" t="s">
+      <c r="G24" s="17"/>
+      <c r="H24" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I24" s="14" t="s">
+      <c r="I24" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J24" s="19" t="s">
+      <c r="J24" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="16" t="s">
+      <c r="B25" s="16"/>
+      <c r="C25" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="E25" s="17"/>
-      <c r="F25" s="14" t="s">
+      <c r="E25" s="18"/>
+      <c r="F25" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="16"/>
-      <c r="H25" s="18" t="s">
+      <c r="G25" s="17"/>
+      <c r="H25" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I25" s="14" t="s">
+      <c r="I25" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J25" s="19" t="s">
+      <c r="J25" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="16" t="s">
+      <c r="B26" s="16"/>
+      <c r="C26" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="14" t="s">
+      <c r="E26" s="18"/>
+      <c r="F26" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="16"/>
-      <c r="H26" s="18" t="s">
+      <c r="G26" s="17"/>
+      <c r="H26" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I26" s="14" t="s">
+      <c r="I26" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J26" s="19" t="s">
+      <c r="J26" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="16" t="s">
+      <c r="B27" s="16"/>
+      <c r="C27" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="E27" s="17"/>
-      <c r="F27" s="14" t="s">
+      <c r="E27" s="18"/>
+      <c r="F27" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="16"/>
-      <c r="H27" s="18" t="s">
+      <c r="G27" s="17"/>
+      <c r="H27" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I27" s="14" t="s">
+      <c r="I27" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J27" s="19" t="s">
+      <c r="J27" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="16" t="s">
+      <c r="B28" s="16"/>
+      <c r="C28" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="14" t="s">
+      <c r="E28" s="18"/>
+      <c r="F28" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="16"/>
-      <c r="H28" s="18" t="s">
+      <c r="G28" s="17"/>
+      <c r="H28" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I28" s="14" t="s">
+      <c r="I28" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J28" s="19" t="s">
+      <c r="J28" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="16" t="s">
+      <c r="B29" s="16"/>
+      <c r="C29" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="14" t="s">
+      <c r="E29" s="18"/>
+      <c r="F29" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="16"/>
-      <c r="H29" s="18" t="s">
+      <c r="G29" s="17"/>
+      <c r="H29" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I29" s="14" t="s">
+      <c r="I29" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J29" s="19" t="s">
+      <c r="J29" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="16" t="s">
+      <c r="B30" s="16"/>
+      <c r="C30" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="14" t="s">
+      <c r="E30" s="18"/>
+      <c r="F30" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G30" s="16"/>
-      <c r="H30" s="18" t="s">
+      <c r="G30" s="17"/>
+      <c r="H30" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I30" s="14" t="s">
+      <c r="I30" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J30" s="19" t="s">
+      <c r="J30" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="16" t="s">
+      <c r="B31" s="16"/>
+      <c r="C31" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="E31" s="17"/>
-      <c r="F31" s="14" t="s">
+      <c r="E31" s="18"/>
+      <c r="F31" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="16"/>
-      <c r="H31" s="18" t="s">
+      <c r="G31" s="17"/>
+      <c r="H31" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I31" s="14" t="s">
+      <c r="I31" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J31" s="19" t="s">
+      <c r="J31" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="16" t="s">
+      <c r="B32" s="16"/>
+      <c r="C32" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="E32" s="17"/>
-      <c r="F32" s="14" t="s">
+      <c r="E32" s="18"/>
+      <c r="F32" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G32" s="16"/>
-      <c r="H32" s="18" t="s">
+      <c r="G32" s="17"/>
+      <c r="H32" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I32" s="14" t="s">
+      <c r="I32" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J32" s="19" t="s">
+      <c r="J32" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="16" t="s">
+      <c r="B33" s="16"/>
+      <c r="C33" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E33" s="17"/>
-      <c r="F33" s="14" t="s">
+      <c r="E33" s="18"/>
+      <c r="F33" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="16"/>
-      <c r="H33" s="18" t="s">
+      <c r="G33" s="17"/>
+      <c r="H33" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I33" s="14" t="s">
+      <c r="I33" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J33" s="19" t="s">
+      <c r="J33" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B34" s="15"/>
-      <c r="C34" s="16" t="s">
+      <c r="B34" s="16"/>
+      <c r="C34" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="E34" s="17"/>
-      <c r="F34" s="14" t="s">
+      <c r="E34" s="18"/>
+      <c r="F34" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G34" s="16"/>
-      <c r="H34" s="18" t="s">
+      <c r="G34" s="17"/>
+      <c r="H34" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I34" s="14" t="s">
+      <c r="I34" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J34" s="19" t="s">
+      <c r="J34" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="22" t="s">
+      <c r="B35" s="22"/>
+      <c r="C35" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="D35" s="23" t="n">
+      <c r="D35" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="E35" s="23" t="n">
+      <c r="E35" s="24" t="n">
         <v>10</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="F35" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="G35" s="22" t="s">
+      <c r="G35" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="H35" s="20" t="s">
+      <c r="H35" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="I35" s="20" t="s">
+      <c r="I35" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="J35" s="24" t="s">
+      <c r="J35" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="21"/>
-      <c r="C36" s="22" t="s">
+      <c r="B36" s="22"/>
+      <c r="C36" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="23" t="n">
+      <c r="D36" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="E36" s="23" t="n">
+      <c r="E36" s="24" t="n">
         <v>6</v>
       </c>
-      <c r="F36" s="20" t="s">
+      <c r="F36" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="G36" s="22" t="s">
+      <c r="G36" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H36" s="20" t="s">
+      <c r="H36" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="I36" s="20" t="s">
+      <c r="I36" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="J36" s="24" t="s">
+      <c r="J36" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="20" t="s">
+      <c r="A37" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="22" t="s">
+      <c r="B37" s="22"/>
+      <c r="C37" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="23" t="n">
+      <c r="D37" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="E37" s="23" t="n">
+      <c r="E37" s="24" t="n">
         <v>5</v>
       </c>
-      <c r="F37" s="20" t="s">
+      <c r="F37" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="G37" s="22" t="s">
+      <c r="G37" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="H37" s="20" t="s">
+      <c r="H37" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="I37" s="20" t="s">
+      <c r="I37" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="J37" s="24" t="s">
+      <c r="J37" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="21"/>
-      <c r="C38" s="22" t="s">
+      <c r="B38" s="22"/>
+      <c r="C38" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="23" t="n">
+      <c r="D38" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="E38" s="23" t="n">
+      <c r="E38" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="F38" s="20" t="s">
+      <c r="F38" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="G38" s="22"/>
-      <c r="H38" s="20" t="s">
+      <c r="G38" s="23"/>
+      <c r="H38" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="I38" s="20" t="s">
+      <c r="I38" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="J38" s="24" t="s">
+      <c r="J38" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="20" t="s">
+      <c r="A39" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="22" t="s">
+      <c r="B39" s="22"/>
+      <c r="C39" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="23" t="n">
+      <c r="D39" s="24" t="n">
         <v>5</v>
       </c>
-      <c r="E39" s="23" t="n">
+      <c r="E39" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="F39" s="20" t="s">
+      <c r="F39" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="G39" s="22"/>
-      <c r="H39" s="20" t="s">
+      <c r="G39" s="23"/>
+      <c r="H39" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="I39" s="20" t="s">
+      <c r="I39" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="J39" s="24" t="s">
+      <c r="J39" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="27" t="s">
+      <c r="B40" s="27"/>
+      <c r="C40" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="28" t="n">
+      <c r="D40" s="29" t="n">
         <v>6</v>
       </c>
-      <c r="E40" s="28"/>
-      <c r="F40" s="25" t="s">
+      <c r="E40" s="29"/>
+      <c r="F40" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G40" s="27"/>
-      <c r="H40" s="25" t="s">
+      <c r="G40" s="28"/>
+      <c r="H40" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I40" s="25" t="s">
+      <c r="I40" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J40" s="29" t="s">
+      <c r="J40" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="B41" s="26"/>
-      <c r="C41" s="27" t="s">
+      <c r="B41" s="27"/>
+      <c r="C41" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="28" t="n">
+      <c r="D41" s="29" t="n">
         <v>7</v>
       </c>
-      <c r="E41" s="28"/>
-      <c r="F41" s="25" t="s">
+      <c r="E41" s="29"/>
+      <c r="F41" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G41" s="27"/>
-      <c r="H41" s="25" t="s">
+      <c r="G41" s="28"/>
+      <c r="H41" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I41" s="25" t="s">
+      <c r="I41" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J41" s="29" t="s">
+      <c r="J41" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B42" s="26"/>
-      <c r="C42" s="27" t="s">
+      <c r="B42" s="27"/>
+      <c r="C42" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="28" t="n">
+      <c r="D42" s="29" t="n">
         <v>8</v>
       </c>
-      <c r="E42" s="28"/>
-      <c r="F42" s="25" t="s">
+      <c r="E42" s="29"/>
+      <c r="F42" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G42" s="27"/>
-      <c r="H42" s="25" t="s">
+      <c r="G42" s="28"/>
+      <c r="H42" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I42" s="25" t="s">
+      <c r="I42" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J42" s="29" t="s">
+      <c r="J42" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="26"/>
-      <c r="C43" s="27" t="s">
+      <c r="B43" s="27"/>
+      <c r="C43" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D43" s="28" t="n">
+      <c r="D43" s="29" t="n">
         <v>9</v>
       </c>
-      <c r="E43" s="28"/>
-      <c r="F43" s="25" t="s">
+      <c r="E43" s="29"/>
+      <c r="F43" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G43" s="27"/>
-      <c r="H43" s="25" t="s">
+      <c r="G43" s="28"/>
+      <c r="H43" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I43" s="25" t="s">
+      <c r="I43" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J43" s="29" t="s">
+      <c r="J43" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="26"/>
-      <c r="C44" s="27" t="s">
+      <c r="B44" s="27"/>
+      <c r="C44" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D44" s="28" t="n">
+      <c r="D44" s="29" t="n">
         <v>10</v>
       </c>
-      <c r="E44" s="28"/>
-      <c r="F44" s="25" t="s">
+      <c r="E44" s="29"/>
+      <c r="F44" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G44" s="27"/>
-      <c r="H44" s="25" t="s">
+      <c r="G44" s="28"/>
+      <c r="H44" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I44" s="25" t="s">
+      <c r="I44" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J44" s="29" t="s">
+      <c r="J44" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="25" t="s">
+      <c r="A45" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="26"/>
-      <c r="C45" s="27" t="s">
+      <c r="B45" s="27"/>
+      <c r="C45" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D45" s="28" t="n">
+      <c r="D45" s="29" t="n">
         <v>11</v>
       </c>
-      <c r="E45" s="28"/>
-      <c r="F45" s="25" t="s">
+      <c r="E45" s="29"/>
+      <c r="F45" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G45" s="27"/>
-      <c r="H45" s="25" t="s">
+      <c r="G45" s="28"/>
+      <c r="H45" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I45" s="25" t="s">
+      <c r="I45" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J45" s="29" t="s">
+      <c r="J45" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="25" t="s">
+      <c r="A46" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B46" s="26"/>
-      <c r="C46" s="27" t="s">
+      <c r="B46" s="27"/>
+      <c r="C46" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D46" s="28" t="n">
+      <c r="D46" s="29" t="n">
         <v>12</v>
       </c>
-      <c r="E46" s="28"/>
-      <c r="F46" s="25" t="s">
+      <c r="E46" s="29"/>
+      <c r="F46" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G46" s="27"/>
-      <c r="H46" s="25" t="s">
+      <c r="G46" s="28"/>
+      <c r="H46" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I46" s="25" t="s">
+      <c r="I46" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J46" s="29" t="s">
+      <c r="J46" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="25" t="s">
+      <c r="A47" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B47" s="26"/>
-      <c r="C47" s="27" t="s">
+      <c r="B47" s="27"/>
+      <c r="C47" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D47" s="28" t="n">
+      <c r="D47" s="29" t="n">
         <v>13</v>
       </c>
-      <c r="E47" s="28"/>
-      <c r="F47" s="25" t="s">
+      <c r="E47" s="29"/>
+      <c r="F47" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G47" s="27"/>
-      <c r="H47" s="25" t="s">
+      <c r="G47" s="28"/>
+      <c r="H47" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I47" s="25" t="s">
+      <c r="I47" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J47" s="29" t="s">
+      <c r="J47" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="25" t="s">
+      <c r="A48" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="26"/>
-      <c r="C48" s="27" t="s">
+      <c r="B48" s="27"/>
+      <c r="C48" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="28" t="n">
+      <c r="D48" s="29" t="n">
         <v>14</v>
       </c>
-      <c r="E48" s="28"/>
-      <c r="F48" s="25" t="s">
+      <c r="E48" s="29"/>
+      <c r="F48" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G48" s="27"/>
-      <c r="H48" s="25" t="s">
+      <c r="G48" s="28"/>
+      <c r="H48" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I48" s="25" t="s">
+      <c r="I48" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J48" s="29" t="s">
+      <c r="J48" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B49" s="26"/>
-      <c r="C49" s="27" t="s">
+      <c r="B49" s="27"/>
+      <c r="C49" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D49" s="28" t="n">
+      <c r="D49" s="29" t="n">
         <v>15</v>
       </c>
-      <c r="E49" s="28"/>
-      <c r="F49" s="25" t="s">
+      <c r="E49" s="29"/>
+      <c r="F49" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G49" s="27"/>
-      <c r="H49" s="25" t="s">
+      <c r="G49" s="28"/>
+      <c r="H49" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I49" s="25" t="s">
+      <c r="I49" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J49" s="29" t="s">
+      <c r="J49" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="25" t="s">
+      <c r="A50" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="26"/>
-      <c r="C50" s="27" t="s">
+      <c r="B50" s="27"/>
+      <c r="C50" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D50" s="28" t="n">
-        <v>16</v>
-      </c>
-      <c r="E50" s="28"/>
-      <c r="F50" s="25" t="s">
+      <c r="D50" s="29" t="n">
+        <v>16</v>
+      </c>
+      <c r="E50" s="29"/>
+      <c r="F50" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G50" s="27"/>
-      <c r="H50" s="25" t="s">
+      <c r="G50" s="28"/>
+      <c r="H50" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I50" s="25" t="s">
+      <c r="I50" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J50" s="29" t="s">
+      <c r="J50" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="25" t="s">
+      <c r="A51" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B51" s="26"/>
-      <c r="C51" s="27" t="s">
+      <c r="B51" s="27"/>
+      <c r="C51" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D51" s="28" t="n">
+      <c r="D51" s="29" t="n">
         <v>17</v>
       </c>
-      <c r="E51" s="28"/>
-      <c r="F51" s="25" t="s">
+      <c r="E51" s="29"/>
+      <c r="F51" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G51" s="27"/>
-      <c r="H51" s="25" t="s">
+      <c r="G51" s="28"/>
+      <c r="H51" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I51" s="25" t="s">
+      <c r="I51" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J51" s="29" t="s">
+      <c r="J51" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="25" t="s">
+      <c r="A52" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B52" s="26"/>
-      <c r="C52" s="27" t="s">
+      <c r="B52" s="27"/>
+      <c r="C52" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D52" s="28" t="n">
+      <c r="D52" s="29" t="n">
         <v>18</v>
       </c>
-      <c r="E52" s="28"/>
-      <c r="F52" s="25" t="s">
+      <c r="E52" s="29"/>
+      <c r="F52" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G52" s="27"/>
-      <c r="H52" s="25" t="s">
+      <c r="G52" s="28"/>
+      <c r="H52" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I52" s="25" t="s">
+      <c r="I52" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J52" s="29" t="s">
+      <c r="J52" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="25" t="s">
+      <c r="A53" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="B53" s="26"/>
-      <c r="C53" s="27" t="s">
+      <c r="B53" s="27"/>
+      <c r="C53" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="D53" s="28" t="n">
+      <c r="D53" s="29" t="n">
         <v>19</v>
       </c>
-      <c r="E53" s="28"/>
-      <c r="F53" s="25" t="s">
+      <c r="E53" s="29"/>
+      <c r="F53" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G53" s="27"/>
-      <c r="H53" s="25" t="s">
+      <c r="G53" s="28"/>
+      <c r="H53" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I53" s="25" t="s">
+      <c r="I53" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J53" s="29" t="s">
+      <c r="J53" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="25" t="s">
+      <c r="A54" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="B54" s="26"/>
-      <c r="C54" s="27" t="s">
+      <c r="B54" s="27"/>
+      <c r="C54" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="D54" s="28" t="n">
+      <c r="D54" s="29" t="n">
         <v>20</v>
       </c>
-      <c r="E54" s="28"/>
-      <c r="F54" s="25" t="s">
+      <c r="E54" s="29"/>
+      <c r="F54" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G54" s="27"/>
-      <c r="H54" s="25" t="s">
+      <c r="G54" s="28"/>
+      <c r="H54" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I54" s="25" t="s">
+      <c r="I54" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J54" s="29" t="s">
+      <c r="J54" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="25" t="s">
+      <c r="A55" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B55" s="26"/>
-      <c r="C55" s="27" t="s">
+      <c r="B55" s="27"/>
+      <c r="C55" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="D55" s="28" t="n">
+      <c r="D55" s="29" t="n">
         <v>21</v>
       </c>
-      <c r="E55" s="28"/>
-      <c r="F55" s="25" t="s">
+      <c r="E55" s="29"/>
+      <c r="F55" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G55" s="27"/>
-      <c r="H55" s="25" t="s">
+      <c r="G55" s="28"/>
+      <c r="H55" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I55" s="25" t="s">
+      <c r="I55" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J55" s="29" t="s">
+      <c r="J55" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="25" t="s">
+      <c r="A56" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="B56" s="26"/>
-      <c r="C56" s="27" t="s">
+      <c r="B56" s="27"/>
+      <c r="C56" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="D56" s="28" t="n">
+      <c r="D56" s="29" t="n">
         <v>22</v>
       </c>
-      <c r="E56" s="28"/>
-      <c r="F56" s="25" t="s">
+      <c r="E56" s="29"/>
+      <c r="F56" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G56" s="27"/>
-      <c r="H56" s="25" t="s">
+      <c r="G56" s="28"/>
+      <c r="H56" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I56" s="25" t="s">
+      <c r="I56" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J56" s="29" t="s">
+      <c r="J56" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="25" t="s">
+      <c r="A57" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B57" s="26"/>
-      <c r="C57" s="27" t="s">
+      <c r="B57" s="27"/>
+      <c r="C57" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="D57" s="28" t="n">
+      <c r="D57" s="29" t="n">
         <v>23</v>
       </c>
-      <c r="E57" s="28"/>
-      <c r="F57" s="25" t="s">
+      <c r="E57" s="29"/>
+      <c r="F57" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G57" s="27"/>
-      <c r="H57" s="25" t="s">
+      <c r="G57" s="28"/>
+      <c r="H57" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I57" s="25" t="s">
+      <c r="I57" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J57" s="29" t="s">
+      <c r="J57" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="25" t="s">
+      <c r="A58" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B58" s="26"/>
-      <c r="C58" s="27" t="s">
+      <c r="B58" s="27"/>
+      <c r="C58" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="D58" s="28" t="n">
+      <c r="D58" s="29" t="n">
         <v>24</v>
       </c>
-      <c r="E58" s="28"/>
-      <c r="F58" s="25" t="s">
+      <c r="E58" s="29"/>
+      <c r="F58" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G58" s="27"/>
-      <c r="H58" s="25" t="s">
+      <c r="G58" s="28"/>
+      <c r="H58" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I58" s="25" t="s">
+      <c r="I58" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J58" s="29" t="s">
+      <c r="J58" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="25" t="s">
+      <c r="A59" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B59" s="26"/>
-      <c r="C59" s="27" t="s">
+      <c r="B59" s="27"/>
+      <c r="C59" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D59" s="28" t="n">
+      <c r="D59" s="29" t="n">
         <v>25</v>
       </c>
-      <c r="E59" s="28"/>
-      <c r="F59" s="25" t="s">
+      <c r="E59" s="29"/>
+      <c r="F59" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G59" s="27"/>
-      <c r="H59" s="25" t="s">
+      <c r="G59" s="28"/>
+      <c r="H59" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I59" s="25" t="s">
+      <c r="I59" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J59" s="29" t="s">
+      <c r="J59" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="25" t="s">
+      <c r="A60" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="26"/>
-      <c r="C60" s="27" t="s">
+      <c r="B60" s="27"/>
+      <c r="C60" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D60" s="28" t="n">
+      <c r="D60" s="29" t="n">
         <v>26</v>
       </c>
-      <c r="E60" s="28"/>
-      <c r="F60" s="25" t="s">
+      <c r="E60" s="29"/>
+      <c r="F60" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G60" s="27"/>
-      <c r="H60" s="25" t="s">
+      <c r="G60" s="28"/>
+      <c r="H60" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I60" s="25" t="s">
+      <c r="I60" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J60" s="29" t="s">
+      <c r="J60" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="25" t="s">
+      <c r="A61" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="26"/>
-      <c r="C61" s="27" t="s">
+      <c r="B61" s="27"/>
+      <c r="C61" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D61" s="28" t="n">
+      <c r="D61" s="29" t="n">
         <v>27</v>
       </c>
-      <c r="E61" s="28"/>
-      <c r="F61" s="25" t="s">
+      <c r="E61" s="29"/>
+      <c r="F61" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G61" s="27"/>
-      <c r="H61" s="25" t="s">
+      <c r="G61" s="28"/>
+      <c r="H61" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I61" s="25" t="s">
+      <c r="I61" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J61" s="29" t="s">
+      <c r="J61" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="25" t="s">
+      <c r="A62" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="B62" s="26"/>
-      <c r="C62" s="27" t="s">
+      <c r="B62" s="27"/>
+      <c r="C62" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D62" s="28" t="n">
+      <c r="D62" s="29" t="n">
         <v>28</v>
       </c>
-      <c r="E62" s="28"/>
-      <c r="F62" s="25" t="s">
+      <c r="E62" s="29"/>
+      <c r="F62" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G62" s="27"/>
-      <c r="H62" s="25" t="s">
+      <c r="G62" s="28"/>
+      <c r="H62" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I62" s="25" t="s">
+      <c r="I62" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J62" s="29" t="s">
+      <c r="J62" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="25" t="s">
+      <c r="A63" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="B63" s="26"/>
-      <c r="C63" s="27" t="s">
+      <c r="B63" s="27"/>
+      <c r="C63" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="D63" s="28" t="n">
+      <c r="D63" s="29" t="n">
         <v>29</v>
       </c>
-      <c r="E63" s="28"/>
-      <c r="F63" s="25" t="s">
+      <c r="E63" s="29"/>
+      <c r="F63" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G63" s="27"/>
-      <c r="H63" s="25" t="s">
+      <c r="G63" s="28"/>
+      <c r="H63" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I63" s="25" t="s">
+      <c r="I63" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J63" s="29" t="s">
+      <c r="J63" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="25" t="s">
+      <c r="A64" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="B64" s="26"/>
-      <c r="C64" s="27" t="s">
+      <c r="B64" s="27"/>
+      <c r="C64" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="D64" s="28" t="n">
+      <c r="D64" s="29" t="n">
         <v>30</v>
       </c>
-      <c r="E64" s="28"/>
-      <c r="F64" s="25" t="s">
+      <c r="E64" s="29"/>
+      <c r="F64" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G64" s="27"/>
-      <c r="H64" s="25" t="s">
+      <c r="G64" s="28"/>
+      <c r="H64" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I64" s="25" t="s">
+      <c r="I64" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J64" s="29" t="s">
+      <c r="J64" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="25" t="s">
+      <c r="A65" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="B65" s="26"/>
-      <c r="C65" s="27" t="s">
+      <c r="B65" s="27"/>
+      <c r="C65" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="D65" s="28" t="n">
+      <c r="D65" s="29" t="n">
         <v>31</v>
       </c>
-      <c r="E65" s="28"/>
-      <c r="F65" s="25" t="s">
+      <c r="E65" s="29"/>
+      <c r="F65" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G65" s="27"/>
-      <c r="H65" s="25" t="s">
+      <c r="G65" s="28"/>
+      <c r="H65" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I65" s="25" t="s">
+      <c r="I65" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J65" s="29" t="s">
+      <c r="J65" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="25" t="s">
+      <c r="A66" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="B66" s="26"/>
-      <c r="C66" s="27" t="s">
+      <c r="B66" s="27"/>
+      <c r="C66" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="D66" s="28" t="n">
+      <c r="D66" s="29" t="n">
         <v>32</v>
       </c>
-      <c r="E66" s="28"/>
-      <c r="F66" s="25" t="s">
+      <c r="E66" s="29"/>
+      <c r="F66" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G66" s="27"/>
-      <c r="H66" s="25" t="s">
+      <c r="G66" s="28"/>
+      <c r="H66" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I66" s="25" t="s">
+      <c r="I66" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J66" s="29" t="s">
+      <c r="J66" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="25" t="s">
+      <c r="A67" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="B67" s="26"/>
-      <c r="C67" s="27" t="s">
+      <c r="B67" s="27"/>
+      <c r="C67" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="D67" s="28" t="n">
+      <c r="D67" s="29" t="n">
         <v>33</v>
       </c>
-      <c r="E67" s="28"/>
-      <c r="F67" s="25" t="s">
+      <c r="E67" s="29"/>
+      <c r="F67" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G67" s="27"/>
-      <c r="H67" s="25" t="s">
+      <c r="G67" s="28"/>
+      <c r="H67" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I67" s="25" t="s">
+      <c r="I67" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J67" s="29" t="s">
+      <c r="J67" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="25" t="s">
+      <c r="A68" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B68" s="26"/>
-      <c r="C68" s="28" t="n">
+      <c r="B68" s="27"/>
+      <c r="C68" s="29" t="n">
         <v>0</v>
       </c>
-      <c r="D68" s="28" t="n">
+      <c r="D68" s="29" t="n">
         <v>34</v>
       </c>
-      <c r="E68" s="28"/>
-      <c r="F68" s="25" t="s">
+      <c r="E68" s="29"/>
+      <c r="F68" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="G68" s="27"/>
-      <c r="H68" s="25" t="s">
+      <c r="G68" s="28"/>
+      <c r="H68" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="I68" s="25" t="s">
+      <c r="I68" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J68" s="29" t="s">
+      <c r="J68" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" s="36" customFormat="true" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B69" s="32"/>
+      <c r="C69" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="E69" s="24" t="n">
+        <v>10</v>
+      </c>
+      <c r="F69" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G69" s="34" t="n">
+        <v>25</v>
+      </c>
+      <c r="H69" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="I69" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="J69" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K69" s="35"/>
+    </row>
+    <row r="70" s="36" customFormat="true" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="B70" s="32"/>
+      <c r="C70" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D70" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="E70" s="24" t="n">
+        <v>6</v>
+      </c>
+      <c r="F70" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G70" s="34" t="n">
+        <v>15</v>
+      </c>
+      <c r="H70" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="I70" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="J70" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K70" s="35"/>
+    </row>
+    <row r="71" s="36" customFormat="true" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B71" s="32"/>
+      <c r="C71" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D71" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="E71" s="24" t="n">
+        <v>5</v>
+      </c>
+      <c r="F71" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G71" s="34" t="n">
+        <v>10</v>
+      </c>
+      <c r="H71" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="I71" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="J71" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K71" s="35"/>
+    </row>
+    <row r="72" s="36" customFormat="true" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B72" s="32"/>
+      <c r="C72" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D72" s="34" t="n">
+        <v>4</v>
+      </c>
+      <c r="E72" s="24" t="n">
+        <v>4</v>
+      </c>
+      <c r="F72" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G72" s="34"/>
+      <c r="H72" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="I72" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="J72" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K72" s="35"/>
+    </row>
+    <row r="73" s="36" customFormat="true" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B73" s="32"/>
+      <c r="C73" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D73" s="34" t="n">
+        <v>5</v>
+      </c>
+      <c r="E73" s="24" t="n">
+        <v>3</v>
+      </c>
+      <c r="F73" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G73" s="34"/>
+      <c r="H73" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="I73" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="J73" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K73" s="35"/>
+    </row>
+    <row r="74" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B74" s="38"/>
+      <c r="C74" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D74" s="40" t="n">
+        <v>6</v>
+      </c>
+      <c r="E74" s="40"/>
+      <c r="F74" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G74" s="40"/>
+      <c r="H74" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I74" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J74" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B75" s="38"/>
+      <c r="C75" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D75" s="40" t="n">
+        <v>7</v>
+      </c>
+      <c r="E75" s="40"/>
+      <c r="F75" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G75" s="40"/>
+      <c r="H75" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I75" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J75" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="B76" s="38"/>
+      <c r="C76" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D76" s="40" t="n">
+        <v>8</v>
+      </c>
+      <c r="E76" s="40"/>
+      <c r="F76" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G76" s="40"/>
+      <c r="H76" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I76" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J76" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="B77" s="38"/>
+      <c r="C77" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D77" s="40" t="n">
+        <v>9</v>
+      </c>
+      <c r="E77" s="40"/>
+      <c r="F77" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G77" s="40"/>
+      <c r="H77" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I77" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J77" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B78" s="38"/>
+      <c r="C78" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D78" s="40" t="n">
+        <v>10</v>
+      </c>
+      <c r="E78" s="40"/>
+      <c r="F78" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G78" s="40"/>
+      <c r="H78" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I78" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J78" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B79" s="38"/>
+      <c r="C79" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D79" s="40" t="n">
+        <v>11</v>
+      </c>
+      <c r="E79" s="40"/>
+      <c r="F79" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G79" s="40"/>
+      <c r="H79" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I79" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J79" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B80" s="38"/>
+      <c r="C80" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D80" s="40" t="n">
+        <v>12</v>
+      </c>
+      <c r="E80" s="40"/>
+      <c r="F80" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G80" s="40"/>
+      <c r="H80" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I80" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J80" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="B81" s="38"/>
+      <c r="C81" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D81" s="40" t="n">
+        <v>13</v>
+      </c>
+      <c r="E81" s="40"/>
+      <c r="F81" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G81" s="40"/>
+      <c r="H81" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I81" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J81" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B82" s="38"/>
+      <c r="C82" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D82" s="40" t="n">
+        <v>14</v>
+      </c>
+      <c r="E82" s="40"/>
+      <c r="F82" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G82" s="40"/>
+      <c r="H82" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I82" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J82" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B83" s="38"/>
+      <c r="C83" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D83" s="40" t="n">
+        <v>15</v>
+      </c>
+      <c r="E83" s="40"/>
+      <c r="F83" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G83" s="40"/>
+      <c r="H83" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I83" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J83" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B84" s="38"/>
+      <c r="C84" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D84" s="40" t="n">
+        <v>16</v>
+      </c>
+      <c r="E84" s="40"/>
+      <c r="F84" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G84" s="40"/>
+      <c r="H84" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I84" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J84" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B85" s="38"/>
+      <c r="C85" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D85" s="40" t="n">
+        <v>17</v>
+      </c>
+      <c r="E85" s="40"/>
+      <c r="F85" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G85" s="40"/>
+      <c r="H85" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I85" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J85" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B86" s="38"/>
+      <c r="C86" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D86" s="40" t="n">
+        <v>18</v>
+      </c>
+      <c r="E86" s="40"/>
+      <c r="F86" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G86" s="40"/>
+      <c r="H86" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I86" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J86" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="B87" s="38"/>
+      <c r="C87" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D87" s="40" t="n">
+        <v>19</v>
+      </c>
+      <c r="E87" s="40"/>
+      <c r="F87" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G87" s="40"/>
+      <c r="H87" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I87" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J87" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="B88" s="38"/>
+      <c r="C88" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D88" s="40" t="n">
+        <v>20</v>
+      </c>
+      <c r="E88" s="40"/>
+      <c r="F88" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G88" s="40"/>
+      <c r="H88" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I88" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J88" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B89" s="38"/>
+      <c r="C89" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D89" s="40" t="n">
+        <v>21</v>
+      </c>
+      <c r="E89" s="40"/>
+      <c r="F89" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G89" s="40"/>
+      <c r="H89" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I89" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J89" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="B90" s="38"/>
+      <c r="C90" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="D90" s="40" t="n">
+        <v>22</v>
+      </c>
+      <c r="E90" s="40"/>
+      <c r="F90" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G90" s="40"/>
+      <c r="H90" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I90" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J90" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B91" s="38"/>
+      <c r="C91" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="D91" s="40" t="n">
+        <v>23</v>
+      </c>
+      <c r="E91" s="40"/>
+      <c r="F91" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G91" s="40"/>
+      <c r="H91" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I91" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J91" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B92" s="38"/>
+      <c r="C92" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="D92" s="40" t="n">
+        <v>24</v>
+      </c>
+      <c r="E92" s="40"/>
+      <c r="F92" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G92" s="40"/>
+      <c r="H92" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I92" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J92" s="30" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2744,86 +3461,86 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="A1" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
     </row>
     <row r="2" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="A2" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="A3" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
     </row>
     <row r="5" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
     </row>
     <row r="6" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
+      <c r="A6" s="42"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
     </row>
     <row r="7" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
+      <c r="A7" s="42"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
     </row>
     <row r="8" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
+      <c r="A8" s="42"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
     </row>
     <row r="9" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
     </row>
     <row r="10" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2834,4 +3551,295 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:D25"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.97"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>